<commit_message>
fixed min vars in env; added more comments on velero items;
</commit_message>
<xml_diff>
--- a/setup/SizingCalculator.xlsx
+++ b/setup/SizingCalculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAnnable\git\otto_public\setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F710036-248D-4888-8A8B-F13EB6A9B075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9480E1-0225-4925-B512-7FDB2D456DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B6676DDB-47BF-48BB-9114-E599C47D7C71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6676DDB-47BF-48BB-9114-E599C47D7C71}"/>
   </bookViews>
   <sheets>
     <sheet name="DEV" sheetId="1" r:id="rId1"/>
@@ -256,7 +256,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6699AA4-2092-4C18-BD56-AF3687BBC0FD}">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,7 +692,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" s="3">
         <v>8</v>
@@ -752,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E15" s="3">
         <v>6</v>
@@ -772,7 +772,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16" s="3">
         <v>6</v>
@@ -850,7 +850,7 @@
       </c>
       <c r="H19">
         <f>B19*D$12+C19*D$13+D19*D$14+E19*D$15+F19*D$16</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I19">
         <f>MAX(ROUNDUP(G19/B$4,0),ROUNDUP(H19/B$5,0))</f>
@@ -878,7 +878,7 @@
       </c>
       <c r="O19" s="5">
         <f>M19-H19-N19</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -906,7 +906,7 @@
       </c>
       <c r="H20">
         <f>B20*D$12+C20*D$13+D20*D$14+E20*D$15+F20*D$16</f>
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="I20">
         <f>MAX(ROUNDUP(G20/B$4,0),ROUNDUP(H20/B$5,0))</f>
@@ -934,7 +934,7 @@
       </c>
       <c r="O20" s="5">
         <f>M20-H20-N20</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1068,7 +1068,7 @@
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>"DJANGO_MEMORY_MAX="&amp;D12</f>
-        <v>DJANGO_MEMORY_MAX=4</v>
+        <v>DJANGO_MEMORY_MAX=3</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
@@ -1176,7 +1176,7 @@
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>"DJANGODB_MEMORY_MAX="&amp;D15</f>
-        <v>DJANGODB_MEMORY_MAX=4</v>
+        <v>DJANGODB_MEMORY_MAX=3</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
@@ -1212,7 +1212,7 @@
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f>"VECTORDB_MEMORY_MAX="&amp;D16</f>
-        <v>VECTORDB_MEMORY_MAX=4</v>
+        <v>VECTORDB_MEMORY_MAX=3</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
@@ -1230,7 +1230,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CB24FB-F203-4A88-8471-D8DDB2FC2483}">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1339,7 +1341,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" s="3">
         <v>8</v>
@@ -1399,7 +1401,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E15" s="3">
         <v>6</v>
@@ -1419,7 +1421,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16" s="3">
         <v>6</v>
@@ -1497,7 +1499,7 @@
       </c>
       <c r="H19">
         <f>B19*D$12+C19*D$13+D19*D$14+E19*D$15+F19*D$16</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I19">
         <f>MAX(ROUNDUP(G19/B$4,0),ROUNDUP(H19/B$5,0))</f>
@@ -1525,7 +1527,7 @@
       </c>
       <c r="O19" s="5">
         <f>M19-H19-N19</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1553,35 +1555,35 @@
       </c>
       <c r="H20">
         <f>B20*D$12+C20*D$13+D20*D$14+E20*D$15+F20*D$16</f>
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="I20">
         <f>MAX(ROUNDUP(G20/B$4,0),ROUNDUP(H20/B$5,0))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J20">
         <f>I20*B$4+K20</f>
-        <v>22.5</v>
+        <v>18</v>
       </c>
       <c r="K20">
         <f>I20*B$8</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="L20" s="5">
         <f>J20-G20-K20</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M20">
         <f>I20*B$5+N20</f>
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="N20">
         <f>I20*B$9</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O20" s="5">
         <f>M20-H20-N20</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1715,7 +1717,7 @@
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>"DJANGO_MEMORY_MAX="&amp;D12</f>
-        <v>DJANGO_MEMORY_MAX=4</v>
+        <v>DJANGO_MEMORY_MAX=3</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
@@ -1823,7 +1825,7 @@
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>"DJANGODB_MEMORY_MAX="&amp;D15</f>
-        <v>DJANGODB_MEMORY_MAX=4</v>
+        <v>DJANGODB_MEMORY_MAX=3</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
@@ -1859,7 +1861,7 @@
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f>"VECTORDB_MEMORY_MAX="&amp;D16</f>
-        <v>VECTORDB_MEMORY_MAX=4</v>
+        <v>VECTORDB_MEMORY_MAX=3</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: configure AKS cluster with user-assigned managed identity and custom route table
- Created a user-assigned managed identity
- Updated AKS cluster to use the user-assigned managed identity
- Created and associated a custom route table with the AKS subnet
- Granted necessary permissions to the managed identity
- Updated AKS cluster to use the custom route table
</commit_message>
<xml_diff>
--- a/setup/SizingCalculator.xlsx
+++ b/setup/SizingCalculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAnnable\git\otto_public\setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9480E1-0225-4925-B512-7FDB2D456DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE1FC3D-51ED-428F-8546-E492BC3149F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6676DDB-47BF-48BB-9114-E599C47D7C71}"/>
   </bookViews>
@@ -594,7 +594,7 @@
   <dimension ref="A1:O59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,7 +830,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
@@ -846,11 +846,11 @@
       </c>
       <c r="G19">
         <f>B19*B$12+C19*B$13+D19*B$14+E19*B$15+F19*B$16</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H19">
         <f>B19*D$12+C19*D$13+D19*D$14+E19*D$15+F19*D$16</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I19">
         <f>MAX(ROUNDUP(G19/B$4,0),ROUNDUP(H19/B$5,0))</f>
@@ -866,7 +866,7 @@
       </c>
       <c r="L19" s="5">
         <f>J19-G19-K19</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19">
         <f>I19*B$5+N19</f>
@@ -878,7 +878,7 @@
       </c>
       <c r="O19" s="5">
         <f>M19-H19-N19</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1044,7 +1044,7 @@
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>"DJANGO_REPLICAS_MIN="&amp;B19</f>
-        <v>DJANGO_REPLICAS_MIN=1</v>
+        <v>DJANGO_REPLICAS_MIN=2</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -1231,7 +1231,7 @@
   <dimension ref="A1:O59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,7 +1479,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
@@ -1495,11 +1495,11 @@
       </c>
       <c r="G19">
         <f>B19*B$12+C19*B$13+D19*B$14+E19*B$15+F19*B$16</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H19">
         <f>B19*D$12+C19*D$13+D19*D$14+E19*D$15+F19*D$16</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I19">
         <f>MAX(ROUNDUP(G19/B$4,0),ROUNDUP(H19/B$5,0))</f>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="L19" s="5">
         <f>J19-G19-K19</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19">
         <f>I19*B$5+N19</f>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="O19" s="5">
         <f>M19-H19-N19</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1693,7 +1693,7 @@
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>"DJANGO_REPLICAS_MIN="&amp;B19</f>
-        <v>DJANGO_REPLICAS_MIN=1</v>
+        <v>DJANGO_REPLICAS_MIN=2</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
remove corporate ip; bring back private; fixed check secret; added user identity to aks; added private dns zone for aks; added service endpoints to subnets; added nsgs;
</commit_message>
<xml_diff>
--- a/setup/SizingCalculator.xlsx
+++ b/setup/SizingCalculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAnnable\git\otto_public\setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9480E1-0225-4925-B512-7FDB2D456DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F9C43E-3132-434B-A2BF-66C89B0DDAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6676DDB-47BF-48BB-9114-E599C47D7C71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B6676DDB-47BF-48BB-9114-E599C47D7C71}"/>
   </bookViews>
   <sheets>
     <sheet name="DEV" sheetId="1" r:id="rId1"/>
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6699AA4-2092-4C18-BD56-AF3687BBC0FD}">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,7 +830,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
@@ -846,11 +846,11 @@
       </c>
       <c r="G19">
         <f>B19*B$12+C19*B$13+D19*B$14+E19*B$15+F19*B$16</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H19">
         <f>B19*D$12+C19*D$13+D19*D$14+E19*D$15+F19*D$16</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I19">
         <f>MAX(ROUNDUP(G19/B$4,0),ROUNDUP(H19/B$5,0))</f>
@@ -866,7 +866,7 @@
       </c>
       <c r="L19" s="5">
         <f>J19-G19-K19</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19">
         <f>I19*B$5+N19</f>
@@ -878,7 +878,7 @@
       </c>
       <c r="O19" s="5">
         <f>M19-H19-N19</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1044,7 +1044,7 @@
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>"DJANGO_REPLICAS_MIN="&amp;B19</f>
-        <v>DJANGO_REPLICAS_MIN=1</v>
+        <v>DJANGO_REPLICAS_MIN=2</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -1067,8 +1067,8 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f>"DJANGO_MEMORY_MAX="&amp;D12</f>
-        <v>DJANGO_MEMORY_MAX=3</v>
+        <f>"DJANGO_MEMORY_MIN="&amp;D12</f>
+        <v>DJANGO_MEMORY_MIN=3</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
@@ -1103,8 +1103,8 @@
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f>"CELERY_MEMORY_MAX="&amp;D13</f>
-        <v>CELERY_MEMORY_MAX=3</v>
+        <f>"CELERY_MEMORY_MIN="&amp;D13</f>
+        <v>CELERY_MEMORY_MIN=3</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
@@ -1139,8 +1139,8 @@
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f>"REDIS_MEMORY_MAX="&amp;D14</f>
-        <v>REDIS_MEMORY_MAX=1</v>
+        <f>"REDIS_MEMORY_MIN="&amp;D14</f>
+        <v>REDIS_MEMORY_MIN=1</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
@@ -1175,8 +1175,8 @@
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
-        <f>"DJANGODB_MEMORY_MAX="&amp;D15</f>
-        <v>DJANGODB_MEMORY_MAX=3</v>
+        <f>"DJANGODB_MEMORY_MIN="&amp;D15</f>
+        <v>DJANGODB_MEMORY_MIN=3</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
@@ -1211,8 +1211,8 @@
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
-        <f>"VECTORDB_MEMORY_MAX="&amp;D16</f>
-        <v>VECTORDB_MEMORY_MAX=3</v>
+        <f>"VECTORDB_MEMORY_MIN="&amp;D16</f>
+        <v>VECTORDB_MEMORY_MIN=3</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
@@ -1230,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CB24FB-F203-4A88-8471-D8DDB2FC2483}">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,7 +1479,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
@@ -1495,11 +1495,11 @@
       </c>
       <c r="G19">
         <f>B19*B$12+C19*B$13+D19*B$14+E19*B$15+F19*B$16</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H19">
         <f>B19*D$12+C19*D$13+D19*D$14+E19*D$15+F19*D$16</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I19">
         <f>MAX(ROUNDUP(G19/B$4,0),ROUNDUP(H19/B$5,0))</f>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="L19" s="5">
         <f>J19-G19-K19</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19">
         <f>I19*B$5+N19</f>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="O19" s="5">
         <f>M19-H19-N19</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1693,7 +1693,7 @@
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>"DJANGO_REPLICAS_MIN="&amp;B19</f>
-        <v>DJANGO_REPLICAS_MIN=1</v>
+        <v>DJANGO_REPLICAS_MIN=2</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -1716,8 +1716,8 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f>"DJANGO_MEMORY_MAX="&amp;D12</f>
-        <v>DJANGO_MEMORY_MAX=3</v>
+        <f>"DJANGO_MEMORY_MIN="&amp;D12</f>
+        <v>DJANGO_MEMORY_MIN=3</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
@@ -1752,8 +1752,8 @@
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f>"CELERY_MEMORY_MAX="&amp;D13</f>
-        <v>CELERY_MEMORY_MAX=3</v>
+        <f>"CELERY_MEMORY_MIN="&amp;D13</f>
+        <v>CELERY_MEMORY_MIN=3</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
@@ -1788,8 +1788,8 @@
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f>"REDIS_MEMORY_MAX="&amp;D14</f>
-        <v>REDIS_MEMORY_MAX=1</v>
+        <f>"REDIS_MEMORY_MIN="&amp;D14</f>
+        <v>REDIS_MEMORY_MIN=1</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
@@ -1824,8 +1824,8 @@
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
-        <f>"DJANGODB_MEMORY_MAX="&amp;D15</f>
-        <v>DJANGODB_MEMORY_MAX=3</v>
+        <f>"DJANGODB_MEMORY_MIN="&amp;D15</f>
+        <v>DJANGODB_MEMORY_MIN=3</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
@@ -1860,8 +1860,8 @@
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
-        <f>"VECTORDB_MEMORY_MAX="&amp;D16</f>
-        <v>VECTORDB_MEMORY_MAX=3</v>
+        <f>"VECTORDB_MEMORY_MIN="&amp;D16</f>
+        <v>VECTORDB_MEMORY_MIN=3</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>